<commit_message>
Changed the ALASCCA class definitions file following discussions with Markus and co..
</commit_message>
<xml_diff>
--- a/reportgen/assets/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/reportgen/assets/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thowhi/repos/reportgen/reportgen/assets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="12800" windowWidth="24000" windowHeight="12320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MutationTable" sheetId="1" r:id="rId1"/>
@@ -13,6 +18,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="177">
   <si>
     <t>Gene</t>
   </si>
@@ -44,9 +52,6 @@
     <t>ENST00000371953</t>
   </si>
   <si>
-    <t>homozygous_loss</t>
-  </si>
-  <si>
     <t>PIK3R1</t>
   </si>
   <si>
@@ -68,12 +73,6 @@
     <t>542,545,546,1021,1043,1044,1047</t>
   </si>
   <si>
-    <t>38,81,88,106,111,118,344,345,378,420,453,726</t>
-  </si>
-  <si>
-    <t>340:670</t>
-  </si>
-  <si>
     <t>start_lost</t>
   </si>
   <si>
@@ -110,18 +109,9 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>amplification</t>
-  </si>
-  <si>
-    <t>IGF2</t>
-  </si>
-  <si>
     <t>Adjusted PIK3CA, KRAS and NRAS hotspots after findings in Chang et al (Identifying recurrent mutations in cancer reveals widespread lineage diversity and mutational specificity). More stringence on PTEN and PIK3R1 after meeting with group. Added focal amp of IGF2 as (preliminary, pending technical sensitivity) addition to class B.</t>
   </si>
   <si>
-    <t>376,379,452,464,503,560,564,567,573,642</t>
-  </si>
-  <si>
     <t>transcript_ablation</t>
   </si>
   <si>
@@ -551,9 +541,6 @@
     <t>VEP Consequence types are SO terms described at http://www.ensembl.org/info/genome/variation/predicted_data.html#consequences</t>
   </si>
   <si>
-    <t>ENSG00000167244</t>
-  </si>
-  <si>
     <t>Amino_acid_changes</t>
   </si>
   <si>
@@ -563,22 +550,16 @@
     <t>Flag</t>
   </si>
   <si>
-    <t>frameshift_variant,inframe_insertion,inframe_deletion,stop_gained,splice_acceptor_variant,splice_donor_variant</t>
-  </si>
-  <si>
     <t>ALASCCA_CLASS_B_1</t>
   </si>
   <si>
-    <t>ALASCCA_CLASS_B_2</t>
-  </si>
-  <si>
     <t>ALASCCA_CLASS_A</t>
   </si>
   <si>
-    <t>start_lost,stop_gained,frameshift_variant,splice_acceptor_variant,splice_donor_variant,loss_of_heterozygosity</t>
-  </si>
-  <si>
-    <t>p.Cys124Ser,p.Gly129Glu,p.Arg130Gly,p.Arg130Gln</t>
+    <t>frameshift_variant,inframe_insertion,inframe_deletion,start_lost,stop_gained,splice_acceptor_variant,splice_donor_variant,missense_variant</t>
+  </si>
+  <si>
+    <t>frameshift_variant,inframe_insertion,inframe_deletion,start_lost,stop_gained,splice_acceptor_variant,splice_donor_variant,missense_variant,homozygous_loss</t>
   </si>
 </sst>
 </file>
@@ -632,7 +613,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -659,12 +640,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -679,7 +654,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="291">
+  <cellStyleXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -971,8 +946,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -988,11 +965,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1000,7 +973,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1009,7 +982,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="291">
+  <cellStyles count="293">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1155,6 +1128,7 @@
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1300,68 +1274,17 @@
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>169333</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>698605</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>42332</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5549900" y="4741333"/>
-          <a:ext cx="3213205" cy="1015999"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100" cap="sq">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1686,32 +1609,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="139.5" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="29.5" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
     <col min="7" max="7" width="5.33203125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1720,373 +1643,374 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="9" t="s">
-        <v>29</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="10"/>
       <c r="F2" s="9" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I2"/>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>6</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="10" t="s">
-        <v>182</v>
+      <c r="F3" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="10" t="s">
-        <v>181</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>181</v>
+      <c r="B5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>174</v>
       </c>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>181</v>
-      </c>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>181</v>
-      </c>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>181</v>
-      </c>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I8"/>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>183</v>
-      </c>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I9"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I14"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I15"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I16"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I17"/>
     </row>
-    <row r="18" spans="1:9">
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="I22"/>
-    </row>
-    <row r="30" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="E30"/>
+      <c r="I30"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="E31"/>
+      <c r="I31"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="E32"/>
+      <c r="I32"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="E33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="E34"/>
+      <c r="I34"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="E35"/>
+      <c r="I35"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="E36"/>
+      <c r="I36"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="E37"/>
+      <c r="I37"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="E38"/>
+      <c r="I38"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="E39"/>
+      <c r="I39"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="E40"/>
+      <c r="I40"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="E41"/>
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="E42"/>
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="E43"/>
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="E44"/>
+      <c r="I44"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="E45"/>
+      <c r="I45"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="E46"/>
+      <c r="I46"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="E47"/>
+      <c r="I47"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="E48"/>
+      <c r="I48"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="E49"/>
+      <c r="I49"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="E50"/>
+      <c r="I50"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="E51"/>
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="E52"/>
+      <c r="I52"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="E53"/>
+      <c r="I53"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="E54"/>
+      <c r="I54"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="E55"/>
+      <c r="I55"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="E56"/>
+      <c r="I56"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="E57"/>
+      <c r="I57"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="E58"/>
+      <c r="I58"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="E59"/>
+      <c r="I59"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="E60"/>
+      <c r="I60"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="3"/>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="E61"/>
+      <c r="I61"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="E62"/>
+      <c r="I62"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="E63"/>
+      <c r="I63"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="E64"/>
+      <c r="I64"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="E65"/>
+      <c r="I65"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="E66"/>
+      <c r="I66"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="E67"/>
+      <c r="I67"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="3"/>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="E68"/>
+      <c r="I68"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="E69"/>
+      <c r="I69"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="E70"/>
+      <c r="I70"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="E71"/>
+      <c r="I71"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="E72"/>
+      <c r="I72"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="3"/>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="E73"/>
+      <c r="I73"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="3"/>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="E74"/>
+      <c r="I74"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="3"/>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="3"/>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="3"/>
+      <c r="E75"/>
+      <c r="I75"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2098,50 +2022,45 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2153,7 +2072,7 @@
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
@@ -2163,635 +2082,630 @@
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="B3" t="s">
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26">
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26">
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
-      <c r="B7" t="s">
+      <c r="E10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E11" t="s">
         <v>113</v>
       </c>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>119</v>
-      </c>
       <c r="F11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="T13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
         <v>124</v>
       </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
         <v>125</v>
       </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="B15" t="s">
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>54</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>126</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>55</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E18" t="s">
         <v>127</v>
       </c>
-      <c r="F15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="B16" t="s">
+      <c r="F18" t="s">
         <v>56</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
         <v>128</v>
       </c>
-      <c r="D16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
         <v>129</v>
       </c>
-      <c r="F16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="F19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
         <v>130</v>
       </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
         <v>131</v>
       </c>
-      <c r="F17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="F20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
         <v>132</v>
       </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
         <v>133</v>
       </c>
-      <c r="F18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" t="s">
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>134</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E22" t="s">
         <v>135</v>
       </c>
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" t="s">
+      <c r="F22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>136</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D23" t="s">
         <v>66</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E23" t="s">
         <v>137</v>
       </c>
-      <c r="F20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" t="s">
+      <c r="F23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>138</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>68</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E24" t="s">
         <v>139</v>
       </c>
-      <c r="F21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" t="s">
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>140</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>70</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E25" t="s">
         <v>141</v>
       </c>
-      <c r="F22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" t="s">
+      <c r="F25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>142</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>72</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>143</v>
       </c>
-      <c r="F23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" t="s">
+      <c r="F26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>144</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>74</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E27" t="s">
         <v>145</v>
       </c>
-      <c r="F24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" t="s">
+      <c r="F27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
         <v>75</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>146</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>76</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E28" t="s">
         <v>147</v>
       </c>
-      <c r="F25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" t="s">
+      <c r="F28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>77</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>148</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>78</v>
       </c>
-      <c r="E26" t="s">
-        <v>149</v>
-      </c>
-      <c r="F26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" t="s">
+      <c r="C30" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" t="s">
         <v>79</v>
       </c>
-      <c r="C27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>80</v>
       </c>
-      <c r="E27" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" t="s">
+      <c r="C31" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" t="s">
         <v>81</v>
       </c>
-      <c r="C28" t="s">
-        <v>152</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>82</v>
       </c>
-      <c r="E28" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" t="s">
+      <c r="C32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" t="s">
         <v>83</v>
       </c>
-      <c r="C29" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="E32" t="s">
         <v>155</v>
       </c>
-      <c r="F29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="B30" t="s">
+      <c r="F32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>84</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>156</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
         <v>85</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E33" t="s">
         <v>157</v>
       </c>
-      <c r="F30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="B31" t="s">
+      <c r="F33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>86</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" t="s">
         <v>158</v>
       </c>
-      <c r="D31" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" t="s">
         <v>159</v>
       </c>
-      <c r="F31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" t="s">
         <v>160</v>
       </c>
-      <c r="D32" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="F35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
         <v>161</v>
       </c>
-      <c r="F32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="B33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" t="s">
         <v>162</v>
       </c>
-      <c r="D33" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" t="s">
-        <v>163</v>
-      </c>
-      <c r="F33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="B34" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" t="s">
-        <v>162</v>
-      </c>
-      <c r="D34" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" t="s">
-        <v>164</v>
-      </c>
-      <c r="F34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="B35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" t="s">
-        <v>165</v>
-      </c>
-      <c r="D35" t="s">
-        <v>95</v>
-      </c>
-      <c r="E35" t="s">
-        <v>166</v>
-      </c>
-      <c r="F35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="B36" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" t="s">
-        <v>167</v>
-      </c>
-      <c r="D36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" t="s">
-        <v>168</v>
-      </c>
       <c r="F36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>